<commit_message>
fully input access db
</commit_message>
<xml_diff>
--- a/acessinputs/LagerSaldo.xlsx
+++ b/acessinputs/LagerSaldo.xlsx
@@ -383,7 +383,7 @@
       </c>
       <c r="D22">
         <f t="shared" ref="D22:D301" si="1">RANDBETWEEN(0, 10)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -398,7 +398,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -413,7 +413,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -428,7 +428,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
@@ -443,7 +443,7 @@
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
@@ -458,7 +458,7 @@
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -473,7 +473,7 @@
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
@@ -488,7 +488,7 @@
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
@@ -518,7 +518,7 @@
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
@@ -533,7 +533,7 @@
       </c>
       <c r="D32">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -548,7 +548,7 @@
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -563,7 +563,7 @@
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -578,7 +578,7 @@
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -593,7 +593,7 @@
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -608,7 +608,7 @@
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -623,7 +623,7 @@
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -638,7 +638,7 @@
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -653,7 +653,7 @@
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
@@ -668,7 +668,7 @@
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42">
@@ -683,7 +683,7 @@
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
@@ -698,7 +698,7 @@
       </c>
       <c r="D43">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -713,7 +713,7 @@
       </c>
       <c r="D44">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -728,7 +728,7 @@
       </c>
       <c r="D45">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -743,7 +743,7 @@
       </c>
       <c r="D46">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
@@ -758,7 +758,7 @@
       </c>
       <c r="D47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48">
@@ -773,7 +773,7 @@
       </c>
       <c r="D48">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
@@ -788,7 +788,7 @@
       </c>
       <c r="D49">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -818,7 +818,7 @@
       </c>
       <c r="D51">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
@@ -833,7 +833,7 @@
       </c>
       <c r="D52">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53">
@@ -848,7 +848,7 @@
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -863,7 +863,7 @@
       </c>
       <c r="D54">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -878,7 +878,7 @@
       </c>
       <c r="D55">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -893,7 +893,7 @@
       </c>
       <c r="D56">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
@@ -908,7 +908,7 @@
       </c>
       <c r="D57">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58">
@@ -923,7 +923,7 @@
       </c>
       <c r="D58">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59">
@@ -938,7 +938,7 @@
       </c>
       <c r="D59">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60">
@@ -953,7 +953,7 @@
       </c>
       <c r="D60">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61">
@@ -968,7 +968,7 @@
       </c>
       <c r="D61">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -983,7 +983,7 @@
       </c>
       <c r="D62">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63">
@@ -998,7 +998,7 @@
       </c>
       <c r="D63">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="D64">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="D65">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="D66">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="D67">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="D68">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="D69">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D70">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D72">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="D73">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="D74">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="D75">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="D76">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D77">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="D78">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="D79">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="D80">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="D81">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D82">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="D83">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="D84">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="D85">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="D86">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="D88">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="D89">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="D90">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="D91">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="D92">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D94">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="D95">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="D96">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="D97">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="D98">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="D100">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="D101">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="D102">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="D103">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D104">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="D105">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="D106">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="D107">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="D108">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="D109">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="D110">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="D111">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="D112">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="D114">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="D115">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D116">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="D117">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="D118">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="D119">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="D120">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="D121">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="D122">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="D124">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="D125">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="D126">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127">
@@ -1958,7 +1958,7 @@
       </c>
       <c r="D127">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128">
@@ -1973,7 +1973,7 @@
       </c>
       <c r="D128">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="D129">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="D130">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="D131">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="D133">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="D134">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="D135">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="D136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="D137">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D138">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="D139">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="D140">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="D141">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142">
@@ -2183,7 +2183,7 @@
       </c>
       <c r="D142">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="D143">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="D144">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="D145">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="D146">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="D147">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="D148">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="149">
@@ -2288,7 +2288,7 @@
       </c>
       <c r="D149">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="D150">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="D151">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="D152">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="D153">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="D154">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="D155">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="D156">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="D157">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="D158">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159">
@@ -2438,7 +2438,7 @@
       </c>
       <c r="D159">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="160">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="D160">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="161">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="D161">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="D162">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="D164">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="D165">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D167">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="D168">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="D169">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="D170">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="171">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="D171">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="D172">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="173">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="D173">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174">
@@ -2663,7 +2663,7 @@
       </c>
       <c r="D174">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="175">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="D175">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="D176">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="D177">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="178">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="D178">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="179">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="D179">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="180">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="D180">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="D181">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
@@ -2783,7 +2783,7 @@
       </c>
       <c r="D182">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="D183">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="184">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="D184">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="D185">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="D186">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="187">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D187">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="D188">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="D189">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="D190">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="191">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="D192">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="193">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="D193">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="D194">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="195">
@@ -2978,7 +2978,7 @@
       </c>
       <c r="D195">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -2993,7 +2993,7 @@
       </c>
       <c r="D196">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="197">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="D197">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="D198">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="199">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="D199">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="200">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="D200">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="D202">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="203">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="D203">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D204">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="205">
@@ -3128,7 +3128,7 @@
       </c>
       <c r="D205">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="206">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="D206">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="207">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="D208">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="209">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="D209">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="210">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="D210">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="D211">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="212">
@@ -3233,7 +3233,7 @@
       </c>
       <c r="D212">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="213">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="D213">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="214">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="D214">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -3278,7 +3278,7 @@
       </c>
       <c r="D215">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="D216">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="217">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="D217">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="218">
@@ -3323,7 +3323,7 @@
       </c>
       <c r="D218">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="D220">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -3368,7 +3368,7 @@
       </c>
       <c r="D221">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222">
@@ -3383,7 +3383,7 @@
       </c>
       <c r="D222">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="D223">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="D224">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="D225">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="D226">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="D227">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="228">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="D228">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="D229">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="D230">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="231">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="D231">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="232">
@@ -3533,7 +3533,7 @@
       </c>
       <c r="D232">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="233">
@@ -3548,7 +3548,7 @@
       </c>
       <c r="D233">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="234">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="D234">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="D235">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="236">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="D236">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="237">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="D237">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="238">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="D238">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="239">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="D239">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="240">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="D240">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="241">
@@ -3668,7 +3668,7 @@
       </c>
       <c r="D241">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -3683,7 +3683,7 @@
       </c>
       <c r="D242">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243">
@@ -3698,7 +3698,7 @@
       </c>
       <c r="D243">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="D244">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="245">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="D245">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="D246">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="247">
@@ -3758,7 +3758,7 @@
       </c>
       <c r="D247">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D248">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="D249">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="250">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="D250">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="251">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="D251">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="252">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="D252">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="D253">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="254">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="D254">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="255">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="D256">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="257">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="D257">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="258">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="D258">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="259">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="D259">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="260">
@@ -3953,7 +3953,7 @@
       </c>
       <c r="D260">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="261">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="D261">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="D262">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="263">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="D263">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="264">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="D264">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="265">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="D265">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="D267">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="268">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="D268">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="269">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="D269">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="D270">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="D271">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="D272">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="D273">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="274">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="D274">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="275">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="D275">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="D276">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="277">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="D277">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="278">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="D278">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="D280">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="281">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="D281">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="D282">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283">
@@ -4298,7 +4298,7 @@
       </c>
       <c r="D283">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="284">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="D284">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="285">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="D285">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286">
@@ -4343,7 +4343,7 @@
       </c>
       <c r="D286">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="287">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="D287">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="288">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="D288">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="289">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="D289">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="290">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="D290">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="291">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="D291">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="292">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="D293">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="294">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="D294">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="295">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="D295">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="D296">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="297">
@@ -4508,7 +4508,7 @@
       </c>
       <c r="D297">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="298">
@@ -4523,7 +4523,7 @@
       </c>
       <c r="D298">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="299">
@@ -4538,7 +4538,7 @@
       </c>
       <c r="D299">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="300">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="D300">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="301">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="D301">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>